<commit_message>
Updated use case 1 and 2
</commit_message>
<xml_diff>
--- a/myQfcProject/mycommon/src/main/resources/Book1.xlsx
+++ b/myQfcProject/mycommon/src/main/resources/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>userid</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>address14</t>
-  </si>
-  <si>
-    <t>user15</t>
   </si>
   <si>
     <t>address15</t>
@@ -426,7 +423,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:C11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,11 +487,11 @@
       <c r="A6">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -502,10 +499,10 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,10 +510,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -524,10 +521,10 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -535,10 +532,10 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,10 +543,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>